<commit_message>
04_pilot, first complete version
</commit_message>
<xml_diff>
--- a/experiments/context_sets.xlsx
+++ b/experiments/context_sets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonyvelasquez/Documents/School/Stanford/QP1/2022 - Autumn/number_precision/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768A6A0-9875-B54D-858C-6383DAE11F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D741FD65-48EF-EB4A-AC1C-A48EFB9069D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="21180" windowHeight="16040" activeTab="3" xr2:uid="{50A77AC9-4DF3-8148-89CD-21D5305E06F1}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="128">
   <si>
     <t xml:space="preserve">Amber and Jeff are planning a picnic in a park where those coming have to bring their own food and picnic blanket. Amber has been collecting RSVPs, and Jeff is wondering how many people they’ll have, so that he can start planning activities for the group. He asks Amber, “How many people said they would come?” </t>
   </si>
@@ -354,13 +354,84 @@
   </si>
   <si>
     <t>Amber and Jeff are resident assistants at a college dorm, and are in charge of putting on a trivia night where they won't play. The way the trivia is set up, they need NUMLIMIT people or less to play. Amber has heard from all the residents about whether they'll attend. Jeff asks her, "How many people said they would come?"</t>
+  </si>
+  <si>
+    <t>agnostic, upper bound</t>
+  </si>
+  <si>
+    <t>agnostic, lower bound</t>
+  </si>
+  <si>
+    <t>Amber and Jeff are trivia planners and are hosting a trivia night. The way the trivia is set up, they need NUMLIMIT people or more to play. Amber has heard from all the residents about whether they'll attend. Jeff asks her, "How many people said they would come?"</t>
+  </si>
+  <si>
+    <t>Amber and Jeff are trivia planners and are hosting a trivia night. The way the trivia is set up, they need NUMLIMIT people or less to play. Amber has heard from all the residents about whether they'll attend. Jeff asks her, "How many people said they would come?"</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are hosting a game night at their house, and will be acting as referees rather than playing themselves. They've planned for their friends to play a new game, which has a limit of twenty-five people. Rachel has heard from all the guests about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are hosting a game night at their house, and will be acting as referees rather than playing themselves. They've planned for their friends to play a new game, which requires at least twenty-five people to play. Rachel has heard from all the guests about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>v0.2</t>
+  </si>
+  <si>
+    <t>agnostic, upper bound
+v0.1</t>
+  </si>
+  <si>
+    <t>agnostic, lower bound
+v0.1</t>
+  </si>
+  <si>
+    <t>Set 2 - Game Night</t>
+  </si>
+  <si>
+    <t>v0.3</t>
+  </si>
+  <si>
+    <t>Amber and Jeff are resident assistants at a college dorm, and are in charge of putting on a trivia night for their residents, where Amber and Jeff won't play. The way the trivia is set up, they need NUMLIMIT people or less to play. Amber has heard from all the residents about whether they'll attend. Jeff asks her, "How many people said they would come?"</t>
+  </si>
+  <si>
+    <t>Amber and Jeff are resident assistants at a college dorm, and are in charge of putting on a trivia night for their residents, where Amber and Jeff won't play. The way the trivia is set up, they need NUMLIMIT people or more to play. Amber has heard from all the residents about whether they'll attend. Jeff asks her, "How many people said they would come?"</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior community, and are hosting a game night for their residents. They've planned for them to play a new game, which requires at least NUMLIMIT people to play. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior community, and are hosting a game night for their residents. They've planned for them to play a new game, which has a limit of NUMLIMIT people. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Set 3 - Extras</t>
+  </si>
+  <si>
+    <t>Set 4 - Chorus</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team for a film and are in charge of casting extras. They need at least NUMLIMIT actors, and can have more. Jill has seen the final number that have been hired. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team for a film and are in charge of casting extras. They can have at most NUMLIMIT actors. Jill has seen the final number that have been hired. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Lauren and Ben are teachers at an elementary school, and are in charge of putting together the chorus for an upcoming play. They need to have NUMLIMIT students or less. After auditions, Lauren has the final count of students who will be joining. Ben asks her, “How many students do we have?”</t>
+  </si>
+  <si>
+    <t>Lauren and Ben are teachers at an elementary school, and are in charge of putting together the chorus for an upcoming play. They need to have NUMLIMIT students or more. After auditions, Lauren has the final count of students who will be joining. Ben asks her, “How many students do we have?”</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They need at least NUMLIMIT actors, and can have more. Jill has seen the final number that have been hired. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They can have at most NUMLIMIT actors. Jill has seen the final number that have been hired. Seth asks her, "How many people do we have?"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -386,6 +457,14 @@
       <name val="Athelas"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Athelas"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -407,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -435,6 +514,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2170,7 +2256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DCE748-6E6E-6E48-9B11-4C5E034B2889}">
   <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -2661,455 +2747,584 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE629B7-7BE3-9549-B13E-E70D2A22B7F2}">
-  <dimension ref="A1:D166"/>
+  <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="67.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="11" customWidth="1"/>
     <col min="4" max="4" width="67.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>11</v>
+      <c r="C3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="3"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="3"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C26" s="4"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C30" s="4"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="9"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="4"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C35" s="4"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C38" s="4"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C39" s="4"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C40" s="4"/>
+      <c r="C40" s="3"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C41" s="4"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C42" s="4"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C43" s="4"/>
+      <c r="C43" s="3"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C44" s="4"/>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C46" s="3"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="9"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="6"/>
+      <c r="C47" s="3"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C54" s="4"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C57" s="4"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C58" s="4"/>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="9"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C61" s="4"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C62" s="4"/>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C63" s="4"/>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C64" s="4"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" s="4"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66" s="4"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C67" s="4"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C68" s="4"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C69" s="4"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C70" s="4"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C71" s="4"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C72" s="4"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C73" s="4"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C74" s="4"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C75" s="4"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C76" s="4"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C78" s="4"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C80" s="4"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C81" s="4"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" s="4"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C83" s="4"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C84" s="4"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C85" s="4"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C86" s="4"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C87" s="4"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C88" s="4"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C89" s="4"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C90" s="4"/>
-    </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C110" s="4"/>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C111" s="4"/>
-    </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C112" s="4"/>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C113" s="4"/>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C114" s="4"/>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C115" s="4"/>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C116" s="4"/>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C117" s="4"/>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C118" s="4"/>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C119" s="4"/>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C120" s="4"/>
-    </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C121" s="4"/>
-    </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C123" s="4"/>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C124" s="4"/>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C125" s="4"/>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C126" s="4"/>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C127" s="4"/>
-    </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C128" s="4"/>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C129" s="4"/>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C130" s="4"/>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C131" s="4"/>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C132" s="4"/>
-    </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C133" s="4"/>
-    </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C134" s="4"/>
-    </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C155" s="4"/>
-    </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C156" s="4"/>
-    </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C157" s="4"/>
-    </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C158" s="4"/>
-    </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C159" s="4"/>
-    </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C160" s="4"/>
-    </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C161" s="4"/>
-    </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C162" s="4"/>
-    </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C163" s="4"/>
-    </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C164" s="4"/>
-    </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C165" s="4"/>
-    </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C166" s="4"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="3"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="3"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="10"/>
+    </row>
+    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="3"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="3"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="3"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="3"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="3"/>
+    </row>
+    <row r="102" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="3"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="3"/>
+    </row>
+    <row r="103" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="3"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="3"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="3"/>
+    </row>
+    <row r="105" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="3"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="3"/>
+    </row>
+    <row r="106" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="3"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="3"/>
+    </row>
+    <row r="107" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="3"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="3"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="3"/>
+    </row>
+    <row r="109" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="3"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="3"/>
+    </row>
+    <row r="110" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="3"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="3"/>
+    </row>
+    <row r="111" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="3"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="3"/>
+    </row>
+    <row r="112" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="3"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="3"/>
+    </row>
+    <row r="113" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="3"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="3"/>
+    </row>
+    <row r="115" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="3"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="3"/>
+    </row>
+    <row r="116" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="3"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="3"/>
+    </row>
+    <row r="117" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="3"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="3"/>
+    </row>
+    <row r="118" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="3"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="3"/>
+    </row>
+    <row r="119" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="3"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="3"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="3"/>
+    </row>
+    <row r="121" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="3"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="3"/>
+    </row>
+    <row r="122" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="3"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="3"/>
+    </row>
+    <row r="123" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="3"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="3"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="3"/>
+    </row>
+    <row r="125" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="3"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="3"/>
+    </row>
+    <row r="126" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="3"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="3"/>
+    </row>
+    <row r="147" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="3"/>
+      <c r="B147" s="7"/>
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="3"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="3"/>
+      <c r="B149" s="7"/>
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="3"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="3"/>
+      <c r="B151" s="7"/>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="3"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="3"/>
+      <c r="B153" s="7"/>
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="3"/>
+      <c r="B154" s="7"/>
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="3"/>
+      <c r="B155" s="7"/>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="3"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="3"/>
+      <c r="B157" s="7"/>
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="3"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final version of 04_pilot
</commit_message>
<xml_diff>
--- a/experiments/context_sets.xlsx
+++ b/experiments/context_sets.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonyvelasquez/Documents/School/Stanford/QP1/2022 - Autumn/number_precision/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D741FD65-48EF-EB4A-AC1C-A48EFB9069D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CE7D22-3C5B-7642-8F40-41C3B1E057CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21180" windowHeight="16040" activeTab="3" xr2:uid="{50A77AC9-4DF3-8148-89CD-21D5305E06F1}"/>
+    <workbookView xWindow="30600" yWindow="-3100" windowWidth="21180" windowHeight="19680" activeTab="4" xr2:uid="{50A77AC9-4DF3-8148-89CD-21D5305E06F1}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.1" sheetId="1" r:id="rId1"/>
     <sheet name="v0.2" sheetId="2" r:id="rId2"/>
     <sheet name="v0.3" sheetId="3" r:id="rId3"/>
-    <sheet name="v0.3 (2)" sheetId="4" r:id="rId4"/>
+    <sheet name="v0.4" sheetId="4" r:id="rId4"/>
+    <sheet name="v0.5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="145">
   <si>
     <t xml:space="preserve">Amber and Jeff are planning a picnic in a park where those coming have to bring their own food and picnic blanket. Amber has been collecting RSVPs, and Jeff is wondering how many people they’ll have, so that he can start planning activities for the group. He asks Amber, “How many people said they would come?” </t>
   </si>
@@ -354,12 +355,6 @@
   </si>
   <si>
     <t>Amber and Jeff are resident assistants at a college dorm, and are in charge of putting on a trivia night where they won't play. The way the trivia is set up, they need NUMLIMIT people or less to play. Amber has heard from all the residents about whether they'll attend. Jeff asks her, "How many people said they would come?"</t>
-  </si>
-  <si>
-    <t>agnostic, upper bound</t>
-  </si>
-  <si>
-    <t>agnostic, lower bound</t>
   </si>
   <si>
     <t>Amber and Jeff are trivia planners and are hosting a trivia night. The way the trivia is set up, they need NUMLIMIT people or more to play. Amber has heard from all the residents about whether they'll attend. Jeff asks her, "How many people said they would come?"</t>
@@ -425,6 +420,63 @@
   </si>
   <si>
     <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They can have at most NUMLIMIT actors. Jill has seen the final number that have been hired. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior center, and are hosting a game night for their residents. They've planned for them to play a new game, which has a limit of NUMLIMIT people. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior center, and are hosting a game night for their residents. They've planned for them to play a new game, which requires at least NUMLIMIT people to play. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They can have at most NUMLIMIT actors. Jill has seen the final number that have been hired and signed contracts. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They need at least NUMLIMIT actors. Jill has seen the final number that have been hired and signed contracts. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Lauren and Ben are teachers at an elementary school, and are in charge of putting together the chorus for an upcoming play. They can have NUMLIMIT students or less. After auditions, Lauren has the final count of students who will be joining. Ben asks her, “How many students do we have?”</t>
+  </si>
+  <si>
+    <t>Lauren and Ben are teachers at an elementary school, and are in charge of putting together the chorus for an upcoming play. They can have NUMLIMIT students or more. After auditions, Lauren has the final count of students who will be joining. Ben asks her, “How many students do we have?”</t>
+  </si>
+  <si>
+    <t>need NUMLIMIT actors at most; can have NUMLIMIT actors at most; can have NUMLIMIT actors or less; need to have NUMLIMIT actors or less/more</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior center, and are hosting a game night for their residents. They've planned for them to play a new game, where no more than NUMLIMIT people can play. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior center, and are hosting a game night for their residents. They've planned for them to play a new game, where NUMLIMIT people or more can play. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They need to have NUMLIMIT actors or less. Jill has seen the final number that have been hired and signed contracts. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They need to have NUMLIMIT actors or more. Jill has seen the final number that have been hired and signed contracts. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior center, and are hosting a game night for their residents. For the game they plan on playing, they can have NUMLIMIT residents or less. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior center, and are hosting a game night for their residents. For the game they plan on playing, they can have NUMLIMIT residents or more. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior center, and are in charge of hosting a game night for their residents. For the game they plan on playing, they can have NUMLIMIT residents or less. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Rachel and Neil are assistants at a senior center, and are in charge of hosting a game night for their residents. For the game they plan on playing, they can have NUMLIMIT residents or more. Rachel has heard from all the residents about whether they'll attend. Neil asks her, “How many people said they would come?”</t>
+  </si>
+  <si>
+    <t>Lauren and Ben are teachers at an elementary school, and are in charge of putting together the chorus for an upcoming play. They can have NUMLIMIT students or less. After the audition process, Lauren has been told by all the parents whether their kids will join. Ben asks her, “How many students do we have?”</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They need to have NUMLIMIT actors or less. After the audition process, Jill has been told the final number that have been hired and signed contracts. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Jill and Seth are on the production team on a film set and are in charge of casting extras. They need to have NUMLIMIT actors or more. After the audition process, Jill has been told the final number that have been hired and signed contracts. Seth asks her, "How many people do we have?"</t>
+  </si>
+  <si>
+    <t>Lauren and Ben are teachers at an elementary school, and are in charge of putting together the chorus for an upcoming play. They can have NUMLIMIT students or more. After the audition process, Lauren has been told by all the parents whether their kids will join. Ben asks her, “How many students do we have?”</t>
   </si>
 </sst>
 </file>
@@ -2749,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE629B7-7BE3-9549-B13E-E70D2A22B7F2}">
   <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2771,47 +2823,49 @@
         <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>104</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C6" s="3"/>
@@ -2828,72 +2882,81 @@
     </row>
     <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>117</v>
+      <c r="D11" s="7" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2908,28 +2971,33 @@
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="C25" s="10"/>
       <c r="D25" s="6"/>
     </row>
@@ -2937,6 +3005,595 @@
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="9"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="3"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="3"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="10"/>
+    </row>
+    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="3"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="3"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="3"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="3"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="3"/>
+    </row>
+    <row r="102" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="3"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="3"/>
+    </row>
+    <row r="103" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="3"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="3"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="3"/>
+    </row>
+    <row r="105" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="3"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="3"/>
+    </row>
+    <row r="106" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="3"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="3"/>
+    </row>
+    <row r="107" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="3"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="3"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="3"/>
+    </row>
+    <row r="109" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="3"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="3"/>
+    </row>
+    <row r="110" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="3"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="3"/>
+    </row>
+    <row r="111" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="3"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="3"/>
+    </row>
+    <row r="112" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="3"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="3"/>
+    </row>
+    <row r="113" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="3"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="3"/>
+    </row>
+    <row r="115" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="3"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="3"/>
+    </row>
+    <row r="116" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="3"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="3"/>
+    </row>
+    <row r="117" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="3"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="3"/>
+    </row>
+    <row r="118" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="3"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="3"/>
+    </row>
+    <row r="119" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="3"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="3"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="3"/>
+    </row>
+    <row r="121" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="3"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="3"/>
+    </row>
+    <row r="122" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="3"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="3"/>
+    </row>
+    <row r="123" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="3"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="3"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="3"/>
+    </row>
+    <row r="125" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="3"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="3"/>
+    </row>
+    <row r="126" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="3"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="3"/>
+    </row>
+    <row r="147" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="3"/>
+      <c r="B147" s="7"/>
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="3"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="3"/>
+      <c r="B149" s="7"/>
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="3"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="3"/>
+      <c r="B151" s="7"/>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="3"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="3"/>
+      <c r="B153" s="7"/>
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="3"/>
+      <c r="B154" s="7"/>
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="3"/>
+      <c r="B155" s="7"/>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="3"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="3"/>
+      <c r="B157" s="7"/>
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="3"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA77DB40-856B-8644-AB7F-F326622F1B4D}">
+  <dimension ref="A1:D158"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="67.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="11" customWidth="1"/>
+    <col min="4" max="4" width="67.6640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="C4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="C5" s="3"/>
+      <c r="D5" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="C6" s="3"/>
+      <c r="D6" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="3"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="C10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="D11" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="D12" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="B25" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
+        <v>132</v>
+      </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
last tweak to 07_pilot--changed attention check answer
</commit_message>
<xml_diff>
--- a/experiments/context_sets.xlsx
+++ b/experiments/context_sets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonyvelasquez/Documents/School/Stanford/QP1/2022 - Autumn/number_precision/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63A24EE-3FC5-0449-BE71-121CFD8A1690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEFDE25-15D0-0246-94B3-21FBD2617998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-3100" windowWidth="21720" windowHeight="16280" activeTab="6" xr2:uid="{50A77AC9-4DF3-8148-89CD-21D5305E06F1}"/>
   </bookViews>
@@ -4719,7 +4719,7 @@
   <dimension ref="A1:D151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>